<commit_message>
UnitList, GamerValues & Use Case Diagram
Opdateret GamerValues med navne og ændret UnitList tilsvarende. Også tilføjet opdateret Use Case Diagram.
</commit_message>
<xml_diff>
--- a/Appendix/GamerValues.xlsx
+++ b/Appendix/GamerValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\odder\OneDrive - Aalborg Universitet\3. Semester\Programming of Complex Software Systems\GitHub\Miniprojekt-PCSS\Appendix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{471AF5CA-41F3-436D-A79D-19A2119FCE02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8088945C-B1A5-4274-8AEA-6594BA135E14}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="8_{471AF5CA-41F3-436D-A79D-19A2119FCE02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CA0DF44A-F2CA-4FF8-9539-E3AA6B3E5BA3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDA3F92B-03A1-421A-A042-3838C57BC28B}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="7">
-  <si>
-    <t>gamer</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>power</t>
   </si>
@@ -44,16 +41,133 @@
     <t>cost</t>
   </si>
   <si>
-    <t>society</t>
-  </si>
-  <si>
-    <t>special</t>
-  </si>
-  <si>
-    <t>delayed</t>
-  </si>
-  <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>HolyGamer</t>
+  </si>
+  <si>
+    <t>TallGamer</t>
+  </si>
+  <si>
+    <t>SamuraiGamer</t>
+  </si>
+  <si>
+    <t>Not-A-Gamer</t>
+  </si>
+  <si>
+    <t>HighSocietyGamer</t>
+  </si>
+  <si>
+    <t>SocietyGamer</t>
+  </si>
+  <si>
+    <t>HackerGamer</t>
+  </si>
+  <si>
+    <t>FrenchGamer</t>
+  </si>
+  <si>
+    <t>DelayedGamer</t>
+  </si>
+  <si>
+    <t>CursedGamer</t>
+  </si>
+  <si>
+    <t>StillAGamer</t>
+  </si>
+  <si>
+    <t>SweatyGamer</t>
+  </si>
+  <si>
+    <t>OrangeGamer</t>
+  </si>
+  <si>
+    <t>ConfusedGamer</t>
+  </si>
+  <si>
+    <t>CowboyGamer</t>
+  </si>
+  <si>
+    <t>AnurognathusGamer</t>
+  </si>
+  <si>
+    <t>SwirlyGamer</t>
+  </si>
+  <si>
+    <t>SexyGamer</t>
+  </si>
+  <si>
+    <t>SushiGamer</t>
+  </si>
+  <si>
+    <t>RevolutionaryGamer</t>
+  </si>
+  <si>
+    <t>Colonioal Gamer</t>
+  </si>
+  <si>
+    <t>MysteriousGamer</t>
+  </si>
+  <si>
+    <t>Dragonborn Gamer</t>
+  </si>
+  <si>
+    <t>FrogGamer</t>
+  </si>
+  <si>
+    <t>PipeGamer</t>
+  </si>
+  <si>
+    <t>VillainGamer</t>
+  </si>
+  <si>
+    <t>HillbillyGamer</t>
+  </si>
+  <si>
+    <t>MathGamer</t>
+  </si>
+  <si>
+    <t>NoseGodGamer</t>
+  </si>
+  <si>
+    <t>YoungGamer</t>
+  </si>
+  <si>
+    <t>PunishedGamer</t>
+  </si>
+  <si>
+    <t>TrueGamer</t>
+  </si>
+  <si>
+    <t>SociallyDistantGamer</t>
+  </si>
+  <si>
+    <t>NordicGamer</t>
+  </si>
+  <si>
+    <t>OneEyedGamer</t>
+  </si>
+  <si>
+    <t>AbstractGamer</t>
+  </si>
+  <si>
+    <t>SpecialGamer</t>
+  </si>
+  <si>
+    <t>LuckyGamer</t>
+  </si>
+  <si>
+    <t>ConstructionGamer</t>
+  </si>
+  <si>
+    <t>CuteSchoolGamer</t>
+  </si>
+  <si>
+    <t>AverageGamer</t>
+  </si>
+  <si>
+    <t>GoldenGamer</t>
   </si>
 </sst>
 </file>
@@ -481,52 +595,52 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3">
         <v>333</v>
@@ -535,7 +649,7 @@
         <v>1500</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E2" s="6">
         <v>499</v>
@@ -544,7 +658,7 @@
         <v>2000</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H2" s="7">
         <v>690</v>
@@ -553,7 +667,7 @@
         <v>2500</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K2" s="8">
         <v>1610</v>
@@ -564,7 +678,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3">
         <v>250</v>
@@ -573,7 +687,7 @@
         <v>1000</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E3" s="6">
         <v>400</v>
@@ -582,7 +696,7 @@
         <v>1750</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H3" s="7">
         <v>500</v>
@@ -591,7 +705,7 @@
         <v>2100</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="K3" s="8">
         <v>1200</v>
@@ -602,7 +716,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3">
         <v>200</v>
@@ -611,7 +725,7 @@
         <v>790</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E4" s="6">
         <v>334</v>
@@ -620,7 +734,7 @@
         <v>1666</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H4" s="7">
         <v>400</v>
@@ -629,7 +743,7 @@
         <v>2077</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K4" s="8">
         <v>999</v>
@@ -640,7 +754,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3">
         <v>169</v>
@@ -649,7 +763,7 @@
         <v>669</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E5" s="6">
         <v>333</v>
@@ -658,7 +772,7 @@
         <v>1600</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H5" s="7">
         <v>300</v>
@@ -667,7 +781,7 @@
         <v>1345</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K5" s="8">
         <v>500</v>
@@ -678,7 +792,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B6" s="9">
         <v>150</v>
@@ -687,7 +801,7 @@
         <v>580</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E6" s="12">
         <v>300</v>
@@ -696,7 +810,7 @@
         <v>1234</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H6" s="13">
         <v>250</v>
@@ -705,7 +819,7 @@
         <v>1100</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K6" s="14">
         <v>100</v>
@@ -716,7 +830,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B7" s="15">
         <v>123</v>
@@ -725,7 +839,7 @@
         <v>456</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E7" s="18">
         <v>250</v>
@@ -734,7 +848,7 @@
         <v>1050</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H7" s="19">
         <v>200</v>
@@ -743,7 +857,7 @@
         <v>850</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K7" s="20">
         <v>0</v>
@@ -754,7 +868,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3">
         <v>100</v>
@@ -763,7 +877,7 @@
         <v>360</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E8" s="6">
         <v>200</v>
@@ -772,7 +886,7 @@
         <v>800</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H8" s="7">
         <v>100</v>
@@ -786,7 +900,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B9" s="3">
         <v>69</v>
@@ -795,7 +909,7 @@
         <v>269</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E9" s="6">
         <v>150</v>
@@ -804,7 +918,7 @@
         <v>600</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H9" s="7">
         <v>-100</v>
@@ -818,7 +932,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3">
         <v>50</v>
@@ -827,7 +941,7 @@
         <v>150</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E10" s="6">
         <v>100</v>
@@ -844,7 +958,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B11" s="9">
         <v>10</v>
@@ -853,7 +967,7 @@
         <v>30</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E11" s="12">
         <v>20</v>
@@ -870,7 +984,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B12" s="15">
         <v>5</v>
@@ -879,13 +993,13 @@
         <v>20</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E12" s="6">
-        <v>-70</v>
+        <v>-25</v>
       </c>
       <c r="F12" s="6">
-        <v>-210</v>
+        <v>-75</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
@@ -896,7 +1010,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
@@ -905,13 +1019,13 @@
         <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E13" s="6">
-        <v>-25</v>
+        <v>-70</v>
       </c>
       <c r="F13" s="6">
-        <v>-75</v>
+        <v>-210</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -922,7 +1036,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -942,7 +1056,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B15" s="3">
         <v>-10</v>
@@ -962,7 +1076,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B16" s="9">
         <v>-30</v>
@@ -982,7 +1096,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B17" s="3">
         <v>-50</v>
@@ -1300,18 +1414,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1334,18 +1448,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EF52F9A-11EA-4675-8E03-08F0163D80EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{082627A2-7EF8-46DC-8FEB-481A25C53EA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EF52F9A-11EA-4675-8E03-08F0163D80EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>